<commit_message>
Update Ienumerable vs Iqueryable xls
</commit_message>
<xml_diff>
--- a/IEnumerable vs IQueryable.xlsx
+++ b/IEnumerable vs IQueryable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnas_Vaiceliunas\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Arnas_Vaiceliunas\Documents\repos\.net-int-TASK5-extra-mile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088D30DF-71C3-4B8F-8861-DF7E59EA1E6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E16A14E-B6A7-4BF9-883A-A2D6D3DB768A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4905" windowWidth="29040" windowHeight="17640" xr2:uid="{F49006DF-E021-438F-8CD1-2DB5B10DF5B9}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F49006DF-E021-438F-8CD1-2DB5B10DF5B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Iqueryable operations</t>
   </si>
@@ -160,32 +160,11 @@
             var elem = result.First();</t>
   </si>
   <si>
-    <t xml:space="preserve">              var result = _context.Services.Where(t =&gt; t.Port &gt; 10).AsQueryable();
-            var res = result.ToList();</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     SELECT s.Id, s.MaintainerEmail, s.Name, s.Port
-              FROM Service AS s
-              WHERE s.Port &gt; 10</t>
-  </si>
-  <si>
     <t>SELECT s.Id, s.MaintainerEmail, s.Name, s.Port
               FROM Service AS s
               WHERE s.Port &gt; 10</t>
   </si>
   <si>
-    <t xml:space="preserve">            var result = _context.Services.Where(t =&gt; t.Port &gt; 10).AsEnumerable();
-            var res = result.ToList();</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            var result = _context.Services.Select(t =&gt; t.Port).AsEnumerable();
-            var res = result.ToList();</t>
-  </si>
-  <si>
-    <t>SELECT [s].[Port]
-      FROM [Service] AS [s]</t>
-  </si>
-  <si>
     <t xml:space="preserve">            var result = _context.Services.Select(t =&gt; t.Port).AsQueryable();
             var res = result.ToList();</t>
   </si>
@@ -194,20 +173,28 @@
               FROM Service AS s</t>
   </si>
   <si>
-    <t xml:space="preserve">            var result = _context.Services.Select(t =&gt; t.Port).AsQueryable();
-            var res = result.Max();</t>
-  </si>
-  <si>
     <t>SELECT MAX(s.Port)
               FROM Service AS s</t>
   </si>
   <si>
-    <t xml:space="preserve">              SELECT s.Port
-              FROM Service AS s</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            var result = _context.Services.Select(t =&gt; t.Port).AsEnumerable();
+    <t xml:space="preserve">            var result = _context.Services.AsQueryable().Select(t =&gt; t.Port);
             var res = result.Max();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            var result = _context.Services.AsEnumerable().Select(t =&gt; t.Port);
+            var res = result.Max();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            var result = _context.Services.AsEnumerable().Select(t =&gt; t.Port);
+            var res = result.ToList();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            var result = _context.Services.AsQueryable().Where(t =&gt; t.Port &gt; 10);
+            var res = result.ToList();</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            var result = _context.Services.AsEnumerable().Where(t =&gt; t.Port &gt; 10);
+            var res = result.ToList();</t>
   </si>
 </sst>
 </file>
@@ -260,14 +247,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -585,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{983F56FF-6B58-4BDE-AE6C-DA0F83559D52}">
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -599,147 +586,147 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="128.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="4"/>
-    </row>
-    <row r="8" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="4"/>
+      <c r="D8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="4"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="4"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="4"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:5" ht="54.6" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>